<commit_message>
geen idee eigenlijk. volgens mij iets met bespreekpunten: kan dit project gesloten worden
</commit_message>
<xml_diff>
--- a/Tier.xlsx
+++ b/Tier.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F462EE-0D0A-4613-B3F5-A28A6FB52C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D14A3-4E8B-47FF-BC39-F47360546F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tier 1</t>
   </si>
@@ -42,40 +53,31 @@
     <t xml:space="preserve">Tier 5 </t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Warning</t>
-  </si>
-  <si>
-    <t>&gt;0</t>
-  </si>
-  <si>
-    <t>Sluit bevestiging projectleider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesloten SO </t>
-  </si>
-  <si>
-    <t>Two-check</t>
-  </si>
-  <si>
-    <t>Actiepunt Bram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sluiten </t>
-  </si>
-  <si>
-    <t>Warnings oplossen</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Two-check fixen</t>
+    <t xml:space="preserve">Voorwaarden om te sluiten: </t>
+  </si>
+  <si>
+    <t>Verkooporder gesloten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geen waarschuwingen </t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Geen actiepunten</t>
+  </si>
+  <si>
+    <t>Goedkeuring projectleider</t>
   </si>
 </sst>
 </file>
@@ -394,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H22:H23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,66 +425,62 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+      <c r="B2">
+        <f>4/4</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <f>4/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D2">
+        <f>4/2</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <f>4/1</f>
+        <v>4</v>
+      </c>
+      <c r="F2" t="e">
+        <f>4/0</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>